<commit_message>
docs: UPDATE docs, ADD tUserActivity, tUserRole
</commit_message>
<xml_diff>
--- a/100. LoginSystem Document/210. Data Dictionary.xlsx
+++ b/100. LoginSystem Document/210. Data Dictionary.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" codeName="현재_통합_문서"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C77F6D9-1EA3-4953-A94C-7D8E98A557AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E0801C-1E15-41E1-9CAE-3AC8574911F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17712" windowHeight="10416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23220" yWindow="0" windowWidth="15180" windowHeight="21000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="공통" sheetId="13" r:id="rId1"/>
     <sheet name="로그인" sheetId="14" r:id="rId2"/>
     <sheet name="사용자" sheetId="8" r:id="rId3"/>
+    <sheet name="사용자 활동" sheetId="16" r:id="rId4"/>
+    <sheet name="사용자 역할" sheetId="17" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
   <si>
     <t>DataType</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -157,6 +159,62 @@
   </si>
   <si>
     <t>Name-EN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>활동유형</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>char</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>역할ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>역할유형</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>활동ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin, user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_activity_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_activity_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_act_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_act_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_role_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_role_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUEIDENTIFIER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login, signup</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -505,21 +563,21 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="20" style="2" customWidth="1"/>
     <col min="3" max="3" width="15" style="2" customWidth="1"/>
     <col min="4" max="4" width="9" style="2" customWidth="1"/>
     <col min="5" max="5" width="5" style="2" customWidth="1"/>
     <col min="6" max="6" width="15" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -542,7 +600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -559,7 +617,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -587,23 +645,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68327D69-90B2-45EE-AD8A-897BE0F4CF27}">
   <dimension ref="A2:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="20" style="2" customWidth="1"/>
     <col min="3" max="3" width="15" style="2" customWidth="1"/>
     <col min="4" max="4" width="9" style="2" customWidth="1"/>
     <col min="5" max="5" width="5" style="2" customWidth="1"/>
     <col min="6" max="6" width="15" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -626,7 +684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -646,7 +704,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -663,7 +721,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -697,21 +755,21 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="20" style="2" customWidth="1"/>
     <col min="3" max="3" width="15" style="2" customWidth="1"/>
     <col min="4" max="4" width="9" style="2" customWidth="1"/>
     <col min="5" max="5" width="5" style="2" customWidth="1"/>
     <col min="6" max="6" width="15" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -734,7 +792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -750,11 +808,9 @@
       <c r="E5" s="2">
         <v>32</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -768,7 +824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -780,6 +836,177 @@
       </c>
       <c r="D7" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC7EA22-E66A-4FD9-A98E-032219964DD8}">
+  <dimension ref="A2:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="20" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA10BE6A-5B27-4242-ACBD-F57D539A1336}">
+  <dimension ref="A2:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="20" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9" style="2" customWidth="1"/>
+    <col min="5" max="5" width="5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>